<commit_message>
Migrated old repository files for edited / added files between Sunday and Wednesday.
</commit_message>
<xml_diff>
--- a/documentation/miscellaneous/for Import/Sunday Readings for (advent,lent,christamas,easter).xlsx
+++ b/documentation/miscellaneous/for Import/Sunday Readings for (advent,lent,christamas,easter).xlsx
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ADVENT" sheetId="1" r:id="rId1"/>
-    <sheet name="CHRISTMAS AND MAJOR FEASTS" sheetId="4" r:id="rId2"/>
-    <sheet name="LENT" sheetId="5" r:id="rId3"/>
-    <sheet name="EASTER" sheetId="6" r:id="rId4"/>
+    <sheet name="ADVENT-MODIFIED" sheetId="7" r:id="rId2"/>
+    <sheet name="CHRISTMAS AND MAJOR FEASTS" sheetId="4" r:id="rId3"/>
+    <sheet name="CHRISTMAS -MODIFIED" sheetId="8" r:id="rId4"/>
+    <sheet name="LENT" sheetId="5" r:id="rId5"/>
+    <sheet name="LENT - MODIFIED" sheetId="9" r:id="rId6"/>
+    <sheet name="EASTER" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="503">
   <si>
     <t>Date</t>
   </si>
@@ -278,12 +281,6 @@
     <t>12/24/14</t>
   </si>
   <si>
-    <t>The Nativity of the Lord (Solemnity, Christmas):</t>
-  </si>
-  <si>
-    <t>At the Vigil Mass - ABC</t>
-  </si>
-  <si>
     <t>Isa 62:1-5</t>
   </si>
   <si>
@@ -296,12 +293,6 @@
     <t>(no bibl. ref.)</t>
   </si>
   <si>
-    <t>Matt 1:1-25</t>
-  </si>
-  <si>
-    <t>or 1:18-25</t>
-  </si>
-  <si>
     <t>12/25/14</t>
   </si>
   <si>
@@ -353,24 +344,9 @@
     <t>Heb 1:1-6</t>
   </si>
   <si>
-    <t>John 1:1-18</t>
-  </si>
-  <si>
-    <t>or 1:1-5, 9-14</t>
-  </si>
-  <si>
     <t>12/29/13</t>
   </si>
   <si>
-    <t>Sunday within the Octave of Christmas:</t>
-  </si>
-  <si>
-    <t>The Holy Family of Jesus, Mary, and Joseph</t>
-  </si>
-  <si>
-    <t>(Feast) - ABC</t>
-  </si>
-  <si>
     <t>Sir 3:3-7, 14-17a (diff)</t>
   </si>
   <si>
@@ -404,12 +380,6 @@
     <t>Heb 1:1-2</t>
   </si>
   <si>
-    <t>Luke 2:22-40 </t>
-  </si>
-  <si>
-    <t>or 2:22, 39-40</t>
-  </si>
-  <si>
     <t>12/27/15</t>
   </si>
   <si>
@@ -431,15 +401,6 @@
     <t>Luke 2:41-52</t>
   </si>
   <si>
-    <t>Jan. 1: The Octave Day of Christmas:</t>
-  </si>
-  <si>
-    <t>Solemnity of the Blessed Virgin Mary,</t>
-  </si>
-  <si>
-    <t>the Mother of God - ABC</t>
-  </si>
-  <si>
     <t>Num 6:22-27</t>
   </si>
   <si>
@@ -455,12 +416,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>[Second Sunday after Christmas - ABC]</t>
-  </si>
-  <si>
-    <t>[Note: In the USA, this Sunday is always Epiphany.]</t>
-  </si>
-  <si>
     <t>Sir 24:1-4, 12-16 (diff)</t>
   </si>
   <si>
@@ -473,18 +428,6 @@
     <t>cf. 1 Tim 3:16</t>
   </si>
   <si>
-    <t>John 1:1-18 </t>
-  </si>
-  <si>
-    <t>The Epiphany of the Lord (Solemnity) - ABC</t>
-  </si>
-  <si>
-    <t>[Traditionally celebrated on Jan. 6;</t>
-  </si>
-  <si>
-    <t>in the USA now on the Sunday after Jan. 1]</t>
-  </si>
-  <si>
     <t>Isa 60:1-6</t>
   </si>
   <si>
@@ -500,12 +443,6 @@
     <t>Matt 2:1-12</t>
   </si>
   <si>
-    <t>Sunday after Epiphany:</t>
-  </si>
-  <si>
-    <t>The Baptism of the Lord (Feast) - ABC</t>
-  </si>
-  <si>
     <t>Isa 42:1-4, 6-7</t>
   </si>
   <si>
@@ -545,12 +482,6 @@
     <t>opt: Isa 40:1-5, 9-11 (new)</t>
   </si>
   <si>
-    <t>opt: Ps 104:1b-2, 3-4, 24-25, </t>
-  </si>
-  <si>
-    <t>27-28, 29b-30 (new)</t>
-  </si>
-  <si>
     <t>opt: Titus 2:11-14; 3:4-7 (new)</t>
   </si>
   <si>
@@ -1512,6 +1443,102 @@
   </si>
   <si>
     <t>opt: John 14:15-16, 23b-26 (new)</t>
+  </si>
+  <si>
+    <t>Ps 122:1-2</t>
+  </si>
+  <si>
+    <t>Ps 72:1-2</t>
+  </si>
+  <si>
+    <t>Ps 146:6c-7</t>
+  </si>
+  <si>
+    <t>Ps 24:1-2</t>
+  </si>
+  <si>
+    <t>Ps 80:2-3</t>
+  </si>
+  <si>
+    <t>Ps 85:9ab+10</t>
+  </si>
+  <si>
+    <t>Luke 1:46-48</t>
+  </si>
+  <si>
+    <t>Ps 89:2-3</t>
+  </si>
+  <si>
+    <t>Ps 25:4-5</t>
+  </si>
+  <si>
+    <t>Ps 126:1-2a</t>
+  </si>
+  <si>
+    <t>Isa 12:2-3</t>
+  </si>
+  <si>
+    <t>Phil 1:4-6</t>
+  </si>
+  <si>
+    <t>John 1:6-8</t>
+  </si>
+  <si>
+    <t>Luke 21:25-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isa 61:1 </t>
+  </si>
+  <si>
+    <t>Isa 61:1</t>
+  </si>
+  <si>
+    <t>2 Sam 7:1-5</t>
+  </si>
+  <si>
+    <t>Isa 63:16b-17</t>
+  </si>
+  <si>
+    <t>Isa 35:1-6a</t>
+  </si>
+  <si>
+    <t>Isa 40:1-5</t>
+  </si>
+  <si>
+    <t>Isa 61:1-2a</t>
+  </si>
+  <si>
+    <t>The Nativity of the Lord (Solemnity, Christmas): At the Vigil Mass - ABC</t>
+  </si>
+  <si>
+    <t>Matt 1:1-25 or 1:18-25</t>
+  </si>
+  <si>
+    <t>John 1:1-18 or 1:1-5, 9-14</t>
+  </si>
+  <si>
+    <t>Sunday within the Octave of Christmas: The Holy Family of Jesus, Mary, and Joseph (Feast) - ABC</t>
+  </si>
+  <si>
+    <t>Luke 2:22-40 or 2:22, 39-40</t>
+  </si>
+  <si>
+    <t>Jan. 1: The Octave Day of Christmas: Solemnity of the Blessed Virgin Mary, the Mother of God - ABC</t>
+  </si>
+  <si>
+    <t>[Second Sunday after Christmas - ABC] [Note: In the USA, this Sunday is always Epiphany.]</t>
+  </si>
+  <si>
+    <t>John 1:1-18  or 1:1-5, 9-14</t>
+  </si>
+  <si>
+    <t>The Epiphany of the Lord (Solemnity) - ABC [Traditionally celebrated on Jan. 6; in the USA now on the Sunday after Jan. 1]</t>
+  </si>
+  <si>
+    <t>Sunday after Epiphany: The Baptism of the Lord (Feast) - ABC</t>
+  </si>
+  <si>
+    <t>opt: Ps 104:1b-2, 3-4, 24-25, 27-28, 29b-30 (new)</t>
   </si>
 </sst>
 </file>
@@ -1519,7 +1546,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-14809]yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="[$-14809]yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -1559,8 +1586,8 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1845,7 +1872,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection sqref="A1:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,10 +2232,293 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>471</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>472</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>489</v>
+      </c>
+      <c r="C4" t="s">
+        <v>473</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>485</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>488</v>
+      </c>
+      <c r="C6" t="s">
+        <v>475</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C7" t="s">
+        <v>476</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C8" t="s">
+        <v>477</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>486</v>
+      </c>
+      <c r="F8" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>487</v>
+      </c>
+      <c r="C9" t="s">
+        <v>478</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>479</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>480</v>
+      </c>
+      <c r="D11" t="s">
+        <v>482</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>481</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>486</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>475</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2257,93 +2567,111 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
         <v>85</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>86</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>87</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>88</v>
       </c>
-      <c r="H2" t="s">
+      <c r="D3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>84</v>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" t="s">
+        <v>92</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>103</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>495</v>
       </c>
       <c r="D6" t="s">
         <v>105</v>
@@ -2355,302 +2683,218 @@
         <v>107</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="H6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" t="s">
+        <v>115</v>
+      </c>
       <c r="H7" t="s">
-        <v>109</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B8">
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42005</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>497</v>
+      </c>
+      <c r="D9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" t="s">
         <v>115</v>
       </c>
-      <c r="F8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G8" t="s">
-        <v>117</v>
-      </c>
-      <c r="H8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>112</v>
+      <c r="H9" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>498</v>
+      </c>
+      <c r="D10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>119</v>
+      <c r="A11" s="1">
+        <v>42095</v>
       </c>
       <c r="B11">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>500</v>
       </c>
       <c r="D11" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="F11" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="G11" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H11" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>41974</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>501</v>
+      </c>
+      <c r="D12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" t="s">
+        <v>140</v>
+      </c>
       <c r="H12" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>127</v>
+      <c r="A13" s="1">
+        <v>42309</v>
       </c>
       <c r="B13">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="F13" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="G13" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="H13" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>42005</v>
+        <v>42644</v>
       </c>
       <c r="B14">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="E14" t="s">
-        <v>138</v>
+        <v>502</v>
       </c>
       <c r="F14" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="H14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>142</v>
-      </c>
-      <c r="D17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" t="s">
-        <v>145</v>
-      </c>
-      <c r="F17" t="s">
-        <v>146</v>
-      </c>
-      <c r="G17" t="s">
-        <v>147</v>
-      </c>
-      <c r="H17" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>143</v>
-      </c>
-      <c r="H18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>42095</v>
-      </c>
-      <c r="B19">
-        <v>20</v>
-      </c>
-      <c r="C19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D19" t="s">
         <v>152</v>
-      </c>
-      <c r="E19" t="s">
-        <v>153</v>
-      </c>
-      <c r="F19" t="s">
-        <v>154</v>
-      </c>
-      <c r="G19" t="s">
-        <v>155</v>
-      </c>
-      <c r="H19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>41974</v>
-      </c>
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>157</v>
-      </c>
-      <c r="D22" t="s">
-        <v>159</v>
-      </c>
-      <c r="E22" t="s">
-        <v>160</v>
-      </c>
-      <c r="F22" t="s">
-        <v>161</v>
-      </c>
-      <c r="G22" t="s">
-        <v>162</v>
-      </c>
-      <c r="H22" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>42309</v>
-      </c>
-      <c r="B24">
-        <v>21</v>
-      </c>
-      <c r="C24" t="s">
-        <v>164</v>
-      </c>
-      <c r="D24" t="s">
-        <v>165</v>
-      </c>
-      <c r="E24" t="s">
-        <v>166</v>
-      </c>
-      <c r="F24" t="s">
-        <v>167</v>
-      </c>
-      <c r="G24" t="s">
-        <v>168</v>
-      </c>
-      <c r="H24" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>42644</v>
-      </c>
-      <c r="B25">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>170</v>
-      </c>
-      <c r="D25" t="s">
-        <v>171</v>
-      </c>
-      <c r="E25" t="s">
-        <v>172</v>
-      </c>
-      <c r="F25" t="s">
-        <v>174</v>
-      </c>
-      <c r="G25" t="s">
-        <v>175</v>
-      </c>
-      <c r="H25" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2658,12 +2902,399 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="110.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>495</v>
+      </c>
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42005</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>497</v>
+      </c>
+      <c r="D9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>498</v>
+      </c>
+      <c r="D10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42095</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>500</v>
+      </c>
+      <c r="D11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>41974</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>501</v>
+      </c>
+      <c r="D12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>42309</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" t="s">
+        <v>146</v>
+      </c>
+      <c r="H13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42644</v>
+      </c>
+      <c r="B14">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" t="s">
+        <v>502</v>
+      </c>
+      <c r="F14" t="s">
+        <v>150</v>
+      </c>
+      <c r="G14" t="s">
+        <v>151</v>
+      </c>
+      <c r="H14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,7 +3317,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -2698,7 +3329,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>7</v>
@@ -2712,100 +3343,100 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="D2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="F2" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="G2" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="H2" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="B3">
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="D3" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="E3" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="F3" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="G3" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="H3" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="B4">
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="G4" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="H4" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="B5">
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="E5" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="F5" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="G5" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="H5" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2816,48 +3447,48 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="E6" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="F6" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="G6" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="H6" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="B7">
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="E7" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="F7" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="G7" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="H7" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2868,22 +3499,22 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="D8" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="F8" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="G8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H8" t="s">
         <v>190</v>
-      </c>
-      <c r="H8" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2894,152 +3525,152 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="E9" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="F9" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="G9" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="H9" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="B10">
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="D10" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="E10" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="F10" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="G10" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="H10" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="B11">
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="D11" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="E11" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="F11" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="G11" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="H11" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="B12">
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="D12" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="E12" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="F12" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="G12" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="H12" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="B13">
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="D13" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="E13" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="F13" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="G13" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="H13" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="B14">
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="D14" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="E14" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="F14" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="G14" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="H14" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -3050,132 +3681,132 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="D15" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="E15" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="F15" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="G15" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="H15" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="B16">
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="D16" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E16" t="s">
         <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="G16" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="H16" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="B17">
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="D17" t="s">
+        <v>233</v>
+      </c>
+      <c r="E17" t="s">
+        <v>233</v>
+      </c>
+      <c r="F17" t="s">
+        <v>233</v>
+      </c>
+      <c r="G17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17" t="s">
         <v>257</v>
-      </c>
-      <c r="E17" t="s">
-        <v>257</v>
-      </c>
-      <c r="F17" t="s">
-        <v>257</v>
-      </c>
-      <c r="G17" t="s">
-        <v>257</v>
-      </c>
-      <c r="H17" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="H18" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="H19" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="B20">
         <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="D20" t="s">
+        <v>235</v>
+      </c>
+      <c r="E20" t="s">
+        <v>236</v>
+      </c>
+      <c r="F20" t="s">
+        <v>237</v>
+      </c>
+      <c r="G20" t="s">
+        <v>238</v>
+      </c>
+      <c r="H20" t="s">
         <v>259</v>
-      </c>
-      <c r="E20" t="s">
-        <v>260</v>
-      </c>
-      <c r="F20" t="s">
-        <v>261</v>
-      </c>
-      <c r="G20" t="s">
-        <v>262</v>
-      </c>
-      <c r="H20" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="H21" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="H22" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3183,11 +3814,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -3211,7 +3856,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -3231,28 +3876,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="B2">
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="D2" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="E2" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="F2" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="G2" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="H2" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3260,38 +3905,38 @@
         <v>42039</v>
       </c>
       <c r="C3" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="D5" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="E5" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="F5" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="G5" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="H5" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3301,33 +3946,33 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="B8">
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="D8" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="E8" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="F8" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="G8" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="H8" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3335,138 +3980,138 @@
         <v>42098</v>
       </c>
       <c r="C9" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="D9" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="F9" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="G9" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="C10" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="D10" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="E10" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="G10" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="H10" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="F11" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="E12" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="F12" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="H12" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="E13" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="F13" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="E14" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="H14" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="E15" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="E16" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="E17" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="E18" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="B19">
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="D19" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="E19" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="F19" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="G19" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="H19" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3474,55 +4119,55 @@
         <v>42128</v>
       </c>
       <c r="C20" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="F20" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="H20" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="C21" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="H21" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="B23">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="D23" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="E23" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="F23" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="G23" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="H23" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3533,22 +4178,22 @@
         <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="D24" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="E24" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="F24" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="G24" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="H24" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3559,105 +4204,105 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="D25" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="E25" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="F25" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="G25" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="H25" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="B26">
         <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="D26" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="E26" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="F26" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="G26" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="H26" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="B27">
         <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="D27" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="E27" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="F27" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="G27" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="H27" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="B28">
         <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="D28" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="E28" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="F28" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="G28" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="H28" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3668,27 +4313,27 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="D30" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
       <c r="E30" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
       <c r="F30" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
       <c r="G30" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
       <c r="H30" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3699,74 +4344,74 @@
         <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="D32" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
       <c r="E32" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="F32" t="s">
-        <v>401</v>
+        <v>377</v>
       </c>
       <c r="G32" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="H32" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>402</v>
+        <v>378</v>
       </c>
       <c r="B33">
         <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="D33" t="s">
-        <v>404</v>
+        <v>380</v>
       </c>
       <c r="E33" t="s">
-        <v>405</v>
+        <v>381</v>
       </c>
       <c r="F33" t="s">
-        <v>406</v>
+        <v>382</v>
       </c>
       <c r="G33" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="H33" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
       <c r="B34">
         <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
       <c r="D34" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
       <c r="E34" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
       <c r="F34" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="G34" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="H34" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3777,22 +4422,22 @@
         <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
       <c r="D35" t="s">
-        <v>415</v>
+        <v>391</v>
       </c>
       <c r="E35" t="s">
-        <v>416</v>
+        <v>392</v>
       </c>
       <c r="F35" t="s">
-        <v>417</v>
+        <v>393</v>
       </c>
       <c r="G35" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
       <c r="H35" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3803,87 +4448,87 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
       <c r="D36" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
       <c r="E36" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
       <c r="F36" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="G36" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="H36" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="B37">
         <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="D37" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="E37" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="F37" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="G37" t="s">
-        <v>430</v>
+        <v>406</v>
       </c>
       <c r="H37" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="F38" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>432</v>
+        <v>408</v>
       </c>
       <c r="B39">
         <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="D39" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
       <c r="E39" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
       <c r="F39" t="s">
-        <v>436</v>
+        <v>412</v>
       </c>
       <c r="G39" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
       <c r="H39" t="s">
-        <v>437</v>
+        <v>413</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3894,22 +4539,22 @@
         <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="D41" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="E41" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="F41" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
       <c r="G41" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="H41" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3920,74 +4565,74 @@
         <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>441</v>
+        <v>417</v>
       </c>
       <c r="D42" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
       <c r="E42" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="F42" t="s">
-        <v>444</v>
+        <v>420</v>
       </c>
       <c r="G42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H42" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
       <c r="B43">
         <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>447</v>
+        <v>423</v>
       </c>
       <c r="D43" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
       <c r="E43" t="s">
-        <v>449</v>
+        <v>425</v>
       </c>
       <c r="F43" t="s">
-        <v>450</v>
+        <v>426</v>
       </c>
       <c r="G43" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="H43" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
       <c r="B44">
         <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>453</v>
+        <v>429</v>
       </c>
       <c r="D44" t="s">
-        <v>454</v>
+        <v>430</v>
       </c>
       <c r="E44" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
       <c r="F44" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="G44" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="H44" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3998,22 +4643,22 @@
         <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
       <c r="D45" t="s">
-        <v>459</v>
+        <v>435</v>
       </c>
       <c r="E45" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="F45" t="s">
-        <v>460</v>
+        <v>436</v>
       </c>
       <c r="G45" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="H45" t="s">
-        <v>461</v>
+        <v>437</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -4024,27 +4669,27 @@
         <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>463</v>
+        <v>439</v>
       </c>
       <c r="D46" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="E46" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="F46" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
       <c r="G46" t="s">
-        <v>430</v>
+        <v>406</v>
       </c>
       <c r="H46" t="s">
-        <v>465</v>
+        <v>441</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -4060,22 +4705,22 @@
         <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
       <c r="D49" t="s">
-        <v>467</v>
+        <v>443</v>
       </c>
       <c r="E49" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
       <c r="F49" t="s">
-        <v>469</v>
+        <v>445</v>
       </c>
       <c r="G49" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
       <c r="H49" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -4086,46 +4731,46 @@
         <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="D50" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
       <c r="E50" t="s">
-        <v>479</v>
+        <v>455</v>
       </c>
       <c r="F50" t="s">
-        <v>480</v>
+        <v>456</v>
       </c>
       <c r="G50" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H50" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="C51" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="D51" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="D52" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>478</v>
+        <v>454</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -4136,79 +4781,79 @@
         <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="D54" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="E54" t="s">
-        <v>484</v>
+        <v>460</v>
       </c>
       <c r="F54" t="s">
-        <v>485</v>
+        <v>461</v>
       </c>
       <c r="G54" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H54" t="s">
-        <v>486</v>
+        <v>462</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>487</v>
+        <v>463</v>
       </c>
       <c r="B56">
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>488</v>
+        <v>464</v>
       </c>
       <c r="D56" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="E56" t="s">
-        <v>484</v>
+        <v>460</v>
       </c>
       <c r="F56" t="s">
-        <v>489</v>
+        <v>465</v>
       </c>
       <c r="G56" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H56" t="s">
-        <v>490</v>
+        <v>466</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>491</v>
+        <v>467</v>
       </c>
       <c r="B57">
         <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>492</v>
+        <v>468</v>
       </c>
       <c r="D57" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="E57" t="s">
-        <v>484</v>
+        <v>460</v>
       </c>
       <c r="F57" t="s">
-        <v>493</v>
+        <v>469</v>
       </c>
       <c r="G57" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H57" t="s">
-        <v>494</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Sunday Readings for (advent,lent,christamas,easter).xlsx
</commit_message>
<xml_diff>
--- a/documentation/miscellaneous/for Import/Sunday Readings for (advent,lent,christamas,easter).xlsx
+++ b/documentation/miscellaneous/for Import/Sunday Readings for (advent,lent,christamas,easter).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apc-softdev-it111-05\documentation\miscellaneous\for Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trixia Urquiza\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ADVENT" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="541">
   <si>
     <t>Date</t>
   </si>
@@ -833,12 +833,6 @@
     <t>3/24/16</t>
   </si>
   <si>
-    <t>Holy Thursday: Evening Mass</t>
-  </si>
-  <si>
-    <t>of the Lord's Supper – Years ABC</t>
-  </si>
-  <si>
     <t>Exod 12:1-8, 11-14</t>
   </si>
   <si>
@@ -887,18 +881,6 @@
     <t>The Resurrection of the Lord;</t>
   </si>
   <si>
-    <t>The Easter Vigil in the Holy Night – ABC</t>
-  </si>
-  <si>
-    <t>Use at least three, or up to</t>
-  </si>
-  <si>
-    <t>seven readings from the OT,</t>
-  </si>
-  <si>
-    <t>but always include #3:</t>
-  </si>
-  <si>
     <t>1) Gen 1:1—2:2 or 1, 26-31a</t>
   </si>
   <si>
@@ -923,12 +905,6 @@
     <t>Responses after each OT Reading:</t>
   </si>
   <si>
-    <t>1) Ps 104:1-2, 5-6, 10+12, 13-14, 24+35 </t>
-  </si>
-  <si>
-    <t>   or Ps 33:4-5, 6-7, 12-13, 20-22 </t>
-  </si>
-  <si>
     <t>2) Ps 16:5+8, 9-10, 11</t>
   </si>
   <si>
@@ -956,9 +932,6 @@
     <t>Rom 6:3-11</t>
   </si>
   <si>
-    <t>Response after the Epistle:</t>
-  </si>
-  <si>
     <t>Psalm 118:1-2, 16-17, 22-23</t>
   </si>
   <si>
@@ -1539,6 +1512,147 @@
   </si>
   <si>
     <t>opt: Ps 104:1b-2, 3-4, 24-25, 27-28, 29b-30 (new)</t>
+  </si>
+  <si>
+    <t>Palm Sunday of the Passion of the Lord:At the Procession with Palms – B</t>
+  </si>
+  <si>
+    <t>Palm Sunday of the Passion of the Lord:At the Procession with Palms – C</t>
+  </si>
+  <si>
+    <t>Palm Sunday of the Passion of the Lord:At the Procession with Palms – A</t>
+  </si>
+  <si>
+    <t>Palm Sunday: At the Mass – B</t>
+  </si>
+  <si>
+    <t>Palm Sunday: At the Mass – A</t>
+  </si>
+  <si>
+    <t>Palm Sunday: At the Mass – C</t>
+  </si>
+  <si>
+    <t>Gen 2:7-9</t>
+  </si>
+  <si>
+    <t>Gen 12:1-4a</t>
+  </si>
+  <si>
+    <t>1 Sam 16:1b</t>
+  </si>
+  <si>
+    <t>Gen 22:1-2</t>
+  </si>
+  <si>
+    <t>Exod 20:1-17</t>
+  </si>
+  <si>
+    <t>2 Chr 36:14-16</t>
+  </si>
+  <si>
+    <t>Deut 26:4-10</t>
+  </si>
+  <si>
+    <t>Gen 15:5-12</t>
+  </si>
+  <si>
+    <t>Exod 3:1-8a</t>
+  </si>
+  <si>
+    <t>Josh 5:9a</t>
+  </si>
+  <si>
+    <t>Ps 51:3-4</t>
+  </si>
+  <si>
+    <t>Ps 33:4-5</t>
+  </si>
+  <si>
+    <t>Ps 95:1-2</t>
+  </si>
+  <si>
+    <t>Ps 23:1-3a</t>
+  </si>
+  <si>
+    <t>Ps 130:1-2</t>
+  </si>
+  <si>
+    <t>Ps 116:10+15</t>
+  </si>
+  <si>
+    <t>Ps 19:8</t>
+  </si>
+  <si>
+    <t>Ps 137:1-2</t>
+  </si>
+  <si>
+    <t>Ps 91:1-2</t>
+  </si>
+  <si>
+    <t>Ps 27:1</t>
+  </si>
+  <si>
+    <t>Ps 103:1-2</t>
+  </si>
+  <si>
+    <t>Ps 34:2-3</t>
+  </si>
+  <si>
+    <t>Rom 5:12-19</t>
+  </si>
+  <si>
+    <t>Rom 5:1-2</t>
+  </si>
+  <si>
+    <t>Phil 3:17–4:1 </t>
+  </si>
+  <si>
+    <t>1 Cor 10:1-6</t>
+  </si>
+  <si>
+    <t>John 4:5-42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John 9:1-41 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">John 11:1-45 </t>
+  </si>
+  <si>
+    <t>Luke 15:1-3</t>
+  </si>
+  <si>
+    <t>Matt 21:1-11</t>
+  </si>
+  <si>
+    <t>Luke 19:28-40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark 14:1 – 15:47 </t>
+  </si>
+  <si>
+    <t>Luke 22:14 – 23:56</t>
+  </si>
+  <si>
+    <t>Mark 11:1-10</t>
+  </si>
+  <si>
+    <t>Matt 26:14 – 27:66 </t>
+  </si>
+  <si>
+    <t>Ps 22:8-9</t>
+  </si>
+  <si>
+    <t>Holy Thursday: Evening Mass of the Lord's Supper – Years ABC</t>
+  </si>
+  <si>
+    <t>Easter Sunday: The Resurrection of the Lord; The Easter Vigil in the Holy Night – ABC</t>
+  </si>
+  <si>
+    <t>Use at least three, or up to seven readings from the OT, but always include #3:</t>
+  </si>
+  <si>
+    <t>1) Ps 104:1-2, 5-6, 10+12, 13-14, 24+35    or Ps 33:4-5, 6-7, 12-13, 20-22 </t>
   </si>
 </sst>
 </file>
@@ -1871,8 +1985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2235,7 +2349,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2276,7 +2390,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -2296,7 +2410,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
@@ -2313,16 +2427,16 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="C4" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="F4" t="s">
         <v>23</v>
@@ -2336,7 +2450,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -2353,10 +2467,10 @@
         <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="C6" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
@@ -2373,10 +2487,10 @@
         <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="C7" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="D7" t="s">
         <v>37</v>
@@ -2393,19 +2507,19 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="C8" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="D8" t="s">
         <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="F8" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2413,10 +2527,10 @@
         <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="C9" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
@@ -2436,7 +2550,7 @@
         <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="D10" t="s">
         <v>53</v>
@@ -2445,7 +2559,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2456,10 +2570,10 @@
         <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="D11" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -2476,13 +2590,13 @@
         <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="D12" t="s">
         <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="F12" t="s">
         <v>63</v>
@@ -2496,7 +2610,7 @@
         <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="D13" t="s">
         <v>66</v>
@@ -2567,7 +2681,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="D2" t="s">
         <v>83</v>
@@ -2582,7 +2696,7 @@
         <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2660,7 +2774,7 @@
         <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2671,7 +2785,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="D6" t="s">
         <v>105</v>
@@ -2712,7 +2826,7 @@
         <v>115</v>
       </c>
       <c r="H7" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2749,7 +2863,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="D9" t="s">
         <v>123</v>
@@ -2775,7 +2889,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="D10" t="s">
         <v>128</v>
@@ -2790,7 +2904,7 @@
         <v>131</v>
       </c>
       <c r="H10" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2801,7 +2915,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="D11" t="s">
         <v>132</v>
@@ -2827,7 +2941,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="D12" t="s">
         <v>137</v>
@@ -2885,7 +2999,7 @@
         <v>149</v>
       </c>
       <c r="E14" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="F14" t="s">
         <v>150</v>
@@ -2907,7 +3021,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2954,7 +3068,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="D2" t="s">
         <v>83</v>
@@ -2969,7 +3083,7 @@
         <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3047,7 +3161,7 @@
         <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3058,7 +3172,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="D6" t="s">
         <v>105</v>
@@ -3099,7 +3213,7 @@
         <v>115</v>
       </c>
       <c r="H7" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3136,7 +3250,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="D9" t="s">
         <v>123</v>
@@ -3162,7 +3276,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="D10" t="s">
         <v>128</v>
@@ -3177,7 +3291,7 @@
         <v>131</v>
       </c>
       <c r="H10" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3188,7 +3302,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="D11" t="s">
         <v>132</v>
@@ -3214,7 +3328,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="D12" t="s">
         <v>137</v>
@@ -3272,7 +3386,7 @@
         <v>149</v>
       </c>
       <c r="E14" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="F14" t="s">
         <v>150</v>
@@ -3293,15 +3407,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.140625" customWidth="1"/>
     <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
@@ -3816,14 +3930,576 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>41885</v>
+      </c>
+      <c r="B2">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" t="s">
+        <v>500</v>
+      </c>
+      <c r="E2" t="s">
+        <v>510</v>
+      </c>
+      <c r="F2" t="s">
+        <v>522</v>
+      </c>
+      <c r="G2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" t="s">
+        <v>501</v>
+      </c>
+      <c r="E3" t="s">
+        <v>511</v>
+      </c>
+      <c r="F3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" t="s">
+        <v>512</v>
+      </c>
+      <c r="F4" t="s">
+        <v>523</v>
+      </c>
+      <c r="G4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H4" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" t="s">
+        <v>502</v>
+      </c>
+      <c r="E5" t="s">
+        <v>513</v>
+      </c>
+      <c r="F5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H5" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>41794</v>
+      </c>
+      <c r="B6">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E6" t="s">
+        <v>514</v>
+      </c>
+      <c r="F6" t="s">
+        <v>180</v>
+      </c>
+      <c r="G6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E7" t="s">
+        <v>470</v>
+      </c>
+      <c r="F7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42007</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D8" t="s">
+        <v>503</v>
+      </c>
+      <c r="E8" t="s">
+        <v>515</v>
+      </c>
+      <c r="F8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42219</v>
+      </c>
+      <c r="B9">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D9" t="s">
+        <v>504</v>
+      </c>
+      <c r="E9" t="s">
+        <v>516</v>
+      </c>
+      <c r="F9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>249</v>
+      </c>
+      <c r="D10" t="s">
+        <v>505</v>
+      </c>
+      <c r="E10" t="s">
+        <v>517</v>
+      </c>
+      <c r="F10" t="s">
+        <v>198</v>
+      </c>
+      <c r="G10" t="s">
+        <v>193</v>
+      </c>
+      <c r="H10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>250</v>
+      </c>
+      <c r="D11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E11" t="s">
+        <v>510</v>
+      </c>
+      <c r="F11" t="s">
+        <v>203</v>
+      </c>
+      <c r="G11" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>251</v>
+      </c>
+      <c r="D12" t="s">
+        <v>506</v>
+      </c>
+      <c r="E12" t="s">
+        <v>518</v>
+      </c>
+      <c r="F12" t="s">
+        <v>209</v>
+      </c>
+      <c r="G12" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" t="s">
+        <v>507</v>
+      </c>
+      <c r="E13" t="s">
+        <v>519</v>
+      </c>
+      <c r="F13" t="s">
+        <v>524</v>
+      </c>
+      <c r="G13" t="s">
+        <v>166</v>
+      </c>
+      <c r="H13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" t="s">
+        <v>508</v>
+      </c>
+      <c r="E14" t="s">
+        <v>520</v>
+      </c>
+      <c r="F14" t="s">
+        <v>525</v>
+      </c>
+      <c r="G14" t="s">
+        <v>219</v>
+      </c>
+      <c r="H14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>42524</v>
+      </c>
+      <c r="B15">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>255</v>
+      </c>
+      <c r="D15" t="s">
+        <v>509</v>
+      </c>
+      <c r="E15" t="s">
+        <v>521</v>
+      </c>
+      <c r="F15" t="s">
+        <v>223</v>
+      </c>
+      <c r="G15" t="s">
+        <v>224</v>
+      </c>
+      <c r="H15" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B16">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" t="s">
+        <v>227</v>
+      </c>
+      <c r="E16" t="s">
+        <v>471</v>
+      </c>
+      <c r="F16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G16" t="s">
+        <v>229</v>
+      </c>
+      <c r="H16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>496</v>
+      </c>
+      <c r="D17" t="s">
+        <v>233</v>
+      </c>
+      <c r="E17" t="s">
+        <v>233</v>
+      </c>
+      <c r="F17" t="s">
+        <v>233</v>
+      </c>
+      <c r="G17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>494</v>
+      </c>
+      <c r="H18" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B19">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>495</v>
+      </c>
+      <c r="H19" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>498</v>
+      </c>
+      <c r="D20" t="s">
+        <v>235</v>
+      </c>
+      <c r="E20" t="s">
+        <v>536</v>
+      </c>
+      <c r="F20" t="s">
+        <v>237</v>
+      </c>
+      <c r="G20" t="s">
+        <v>238</v>
+      </c>
+      <c r="H20" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>497</v>
+      </c>
+      <c r="D21" t="s">
+        <v>235</v>
+      </c>
+      <c r="E21" t="s">
+        <v>536</v>
+      </c>
+      <c r="F21" t="s">
+        <v>237</v>
+      </c>
+      <c r="G21" t="s">
+        <v>238</v>
+      </c>
+      <c r="H21" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>499</v>
+      </c>
+      <c r="D22" t="s">
+        <v>235</v>
+      </c>
+      <c r="E22" t="s">
+        <v>536</v>
+      </c>
+      <c r="F22" t="s">
+        <v>237</v>
+      </c>
+      <c r="G22" t="s">
+        <v>238</v>
+      </c>
+      <c r="H22" t="s">
+        <v>533</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3832,8 +4508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3882,31 +4558,28 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
+        <v>537</v>
+      </c>
+      <c r="D2" t="s">
         <v>267</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F2" t="s">
         <v>269</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>270</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>271</v>
-      </c>
-      <c r="G2" t="s">
-        <v>272</v>
-      </c>
-      <c r="H2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42039</v>
       </c>
-      <c r="C3" t="s">
-        <v>268</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3915,28 +4588,28 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E5" t="s">
         <v>276</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>277</v>
-      </c>
-      <c r="E5" t="s">
-        <v>278</v>
-      </c>
-      <c r="F5" t="s">
-        <v>279</v>
       </c>
       <c r="G5" t="s">
         <v>238</v>
       </c>
       <c r="H5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3946,172 +4619,152 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B8">
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>283</v>
+        <v>538</v>
       </c>
       <c r="D8" t="s">
-        <v>286</v>
+        <v>539</v>
       </c>
       <c r="E8" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F8" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="G8" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="H8" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42098</v>
       </c>
-      <c r="C9" t="s">
-        <v>284</v>
-      </c>
-      <c r="D9" t="s">
-        <v>287</v>
-      </c>
       <c r="F9" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="G9" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>282</v>
-      </c>
-      <c r="C10" t="s">
-        <v>285</v>
-      </c>
-      <c r="D10" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="E10" t="s">
-        <v>297</v>
+        <v>540</v>
       </c>
       <c r="G10" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="H10" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>298</v>
-      </c>
-      <c r="F11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E12" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="F12" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="H12" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E13" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="F13" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E14" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="H14" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E15" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E16" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E17" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="E18" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B19">
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D19" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="E19" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="F19" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="G19" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="H19" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -4119,24 +4772,24 @@
         <v>42128</v>
       </c>
       <c r="C20" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F20" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="H20" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>310</v>
+      </c>
+      <c r="C21" t="s">
+        <v>311</v>
+      </c>
+      <c r="H21" t="s">
         <v>319</v>
-      </c>
-      <c r="C21" t="s">
-        <v>320</v>
-      </c>
-      <c r="H21" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4146,28 +4799,28 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B23">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="D23" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="E23" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="F23" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="G23" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="H23" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -4178,22 +4831,22 @@
         <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D24" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="E24" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="F24" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="G24" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="H24" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4204,105 +4857,105 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="D25" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="E25" t="s">
         <v>175</v>
       </c>
       <c r="F25" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="G25" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="H25" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B26">
         <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="D26" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="E26" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="F26" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="G26" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="H26" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B27">
         <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="D27" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="E27" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="F27" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="G27" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="H27" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="B28">
         <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="D28" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="E28" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="F28" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="G28" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="H28" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -4313,22 +4966,22 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="D30" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="E30" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="F30" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="G30" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="H30" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4344,74 +4997,74 @@
         <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D32" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="E32" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="F32" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="G32" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="H32" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="B33">
         <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="D33" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="E33" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="F33" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="G33" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="H33" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="B34">
         <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="D34" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="E34" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="F34" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="G34" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="H34" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -4422,22 +5075,22 @@
         <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="D35" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="E35" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="F35" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="G35" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="H35" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -4448,82 +5101,82 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="D36" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="E36" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="F36" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="G36" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="H36" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="B37">
         <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="D37" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="E37" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="F37" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="G37" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="H37" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="F38" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="B39">
         <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="D39" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="E39" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="F39" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="G39" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="H39" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -4539,22 +5192,22 @@
         <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="D41" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="E41" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="F41" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="G41" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="H41" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -4565,74 +5218,74 @@
         <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="D42" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="E42" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="F42" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="G42" t="s">
         <v>86</v>
       </c>
       <c r="H42" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="B43">
         <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="D43" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="E43" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="F43" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="G43" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="H43" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="B44">
         <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="D44" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="E44" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="F44" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="G44" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H44" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -4643,22 +5296,22 @@
         <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="D45" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="E45" t="s">
         <v>124</v>
       </c>
       <c r="F45" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G45" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="H45" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -4669,27 +5322,27 @@
         <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="D46" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="E46" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="F46" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="G46" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="H46" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -4705,22 +5358,22 @@
         <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="D49" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="E49" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="F49" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="G49" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="H49" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -4731,46 +5384,46 @@
         <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="D50" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="E50" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="F50" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="G50" t="s">
         <v>86</v>
       </c>
       <c r="H50" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="C51" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="D51" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="D52" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -4781,79 +5434,79 @@
         <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="D54" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="E54" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="F54" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="G54" t="s">
         <v>86</v>
       </c>
       <c r="H54" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="B56">
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="D56" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="E56" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="F56" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="G56" t="s">
         <v>86</v>
       </c>
       <c r="H56" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="B57">
         <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="D57" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="E57" t="s">
+        <v>451</v>
+      </c>
+      <c r="F57" t="s">
         <v>460</v>
-      </c>
-      <c r="F57" t="s">
-        <v>469</v>
       </c>
       <c r="G57" t="s">
         <v>86</v>
       </c>
       <c r="H57" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Sunday Readings for (advent,lent,christamas,easter).xlsx for easter season
</commit_message>
<xml_diff>
--- a/documentation/miscellaneous/for Import/Sunday Readings for (advent,lent,christamas,easter).xlsx
+++ b/documentation/miscellaneous/for Import/Sunday Readings for (advent,lent,christamas,easter).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ADVENT" sheetId="1" r:id="rId1"/>
@@ -4598,7 +4598,10 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5372,8 +5375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H57"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>